<commit_message>
update mixed chunks list
</commit_message>
<xml_diff>
--- a/annotated_data/top_10_medicinal_hits/annotations/manually_annotated_chunks/annotated_chunks_list.xlsx
+++ b/annotated_data/top_10_medicinal_hits/annotations/manually_annotated_chunks/annotated_chunks_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rbgkew-my.sharepoint.com/personal/f_civita_kew_org/Documents/Documents/mygithub/MedicinalPlantMining/annotated_data/top_10_medicinal_hits/annotations/manually_annotated_chunks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="14_{FAA565CD-23E9-42EE-9269-EDB9600C0C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{192B5118-B367-49D3-821D-E2ABBABAA92B}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="14_{FAA565CD-23E9-42EE-9269-EDB9600C0C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D0DA499-B3CF-4152-BDE1-47C2537DB921}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1842,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A306" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D234" sqref="D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5175,7 +5175,7 @@
         <v>5</v>
       </c>
       <c r="D233" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E233" t="s">
         <v>440</v>

</xml_diff>